<commit_message>
memory trace and results  added
</commit_message>
<xml_diff>
--- a/artifacts/failure_cases/results/executor_results.xlsx
+++ b/artifacts/failure_cases/results/executor_results.xlsx
@@ -5,18 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\arnav\Documents\VS Code\RAG 12 Week Series\rag-failure-modes\artifacts\failure_cases\questions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\arnav\Documents\VS Code\RAG 12 Week Series\rag-failure-modes\artifacts\failure_cases\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B24AEA3-616E-45E4-8E9C-1182E6F31601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD03B1C-2CF1-4D68-9EB1-9A0E768BAE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Failure Taxonomy" sheetId="1" r:id="rId1"/>
+    <sheet name="Results" sheetId="3" r:id="rId2"/>
+    <sheet name="Questions" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Failure Taxonomy'!$A$1:$E$11</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="58">
   <si>
     <t>FM-E1</t>
   </si>
@@ -112,12 +114,123 @@
   <si>
     <t>Failure Description</t>
   </si>
+  <si>
+    <t>question_id</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>qestion_type</t>
+  </si>
+  <si>
+    <t>question_text</t>
+  </si>
+  <si>
+    <t>expected_retrieval</t>
+  </si>
+  <si>
+    <t>confidence</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Pure Parametric (Retrieval is Harmful)</t>
+  </si>
+  <si>
+    <t>What is self-attention in transformer models?</t>
+  </si>
+  <si>
+    <t>NOOP</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Why does attention allow parallel computation compared to RNNs?</t>
+  </si>
+  <si>
+    <t>Explain the intuition behind scaling dot-product attention by √dk.</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Source Bound Factual (Retrieval is mandatory)</t>
+  </si>
+  <si>
+    <t>What BLEU score did Vaswani et al. report for EN–DE translation?</t>
+  </si>
+  <si>
+    <t>RETRIEVE</t>
+  </si>
+  <si>
+    <t>How many layers were used in the base transformer model in the original paper?</t>
+  </si>
+  <si>
+    <t>What optimizer and learning rate schedule were used in Attention Is All You Need?</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Structural / Section-Specific</t>
+  </si>
+  <si>
+    <t>Summarize Section 3.2 of Attention Is All You Need.</t>
+  </si>
+  <si>
+    <t>According to the paper, what are the main components of the encoder layer?</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Ambiguous Boundary</t>
+  </si>
+  <si>
+    <t>How does the transformer architecture differ from previous sequence models?</t>
+  </si>
+  <si>
+    <t>NOOP (debatable)</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>What evidence supports the claim that attention improves translation quality?</t>
+  </si>
+  <si>
+    <t>RETRIEVE (debatable)</t>
+  </si>
+  <si>
+    <t>planner_action</t>
+  </si>
+  <si>
+    <t>executor_action</t>
+  </si>
+  <si>
+    <t>tool_result_status</t>
+  </si>
+  <si>
+    <t>Skipped</t>
+  </si>
+  <si>
+    <t>Top k = 4</t>
+  </si>
+  <si>
+    <t>failure_mode</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +250,19 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -174,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -196,6 +322,38 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -479,9 +637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -631,4 +787,626 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C959501-0107-412E-B61F-7FB032D52CE1}">
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="11">
+        <v>0</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="11">
+        <v>1</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="11">
+        <v>2</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="11">
+        <v>3</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="11">
+        <v>4</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="11">
+        <v>5</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" s="19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="11">
+        <v>8</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="11">
+        <v>9</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" s="19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="11">
+        <v>10</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="J10" s="19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="11">
+        <v>11</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B016944E-12CD-481C-84CF-07144FC4C7CE}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="11">
+        <v>0</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="11">
+        <v>1</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="11">
+        <v>2</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="11">
+        <v>3</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="11">
+        <v>4</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="11">
+        <v>5</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="11">
+        <v>8</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="11">
+        <v>9</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="11">
+        <v>10</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="11">
+        <v>11</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>